<commit_message>
add fn k_anonymity_dict() to pull indirect identifiers from data dict
</commit_message>
<xml_diff>
--- a/data/dict_nonvalid.xlsx
+++ b/data/dict_nonvalid.xlsx
@@ -1,163 +1,179 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbarks/datadict-cmd/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74235622-CC3C-904C-AF76-219C2E3384F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38120" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
-  <si>
-    <t xml:space="preserve">variable_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">short_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">original</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coded list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, Town A | 1, Town B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cluster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, 1 | 1, 2 | 2, 3 | 3, 4 | 4, 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, City water network piped to household | 1, Direct from canal | 2, Other (specify) | 3, Tank filled by a truck transporting untreated water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, Buying purified water | 1, Untreated water wells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, Female | 1, Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_under_one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, No | 1, Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numeric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">illness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, No | 1, Yes, fever and rash | 2, Yes, other (specify) | 3, Yes, respiratory infection | 4, Yes, watery diarrhoea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ilness_other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, Diarrhea, fever and rash | 1, died before</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oedema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, No | 1, Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">muac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arrived</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_arrived</t>
-  </si>
-  <si>
-    <t xml:space="preserve">departed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_departed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">born</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_born</t>
-  </si>
-  <si>
-    <t xml:space="preserve">died</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_died</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cause_death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, Fever | 1, Other (specify)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cause_death_other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, Cancer | 1, Gunshot | 2, Stroke</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="49">
+  <si>
+    <t>variable_name</t>
+  </si>
+  <si>
+    <t>short_label</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Free text</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>shared</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Coded list</t>
+  </si>
+  <si>
+    <t>0, Town A | 1, Town B</t>
+  </si>
+  <si>
+    <t>cluster</t>
+  </si>
+  <si>
+    <t>0, 1 | 1, 2 | 2, 3 | 3, 4 | 4, 5</t>
+  </si>
+  <si>
+    <t>source_water</t>
+  </si>
+  <si>
+    <t>0, City water network piped to household | 1, Direct from canal | 2, Other (specify) | 3, Tank filled by a truck transporting untreated water</t>
+  </si>
+  <si>
+    <t>0, Buying purified water | 1, Untreated water wells</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>0, Female | 1, Male</t>
+  </si>
+  <si>
+    <t>age_under_one</t>
+  </si>
+  <si>
+    <t>0, No | 1, Yes</t>
+  </si>
+  <si>
+    <t>age_months</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>age_years</t>
+  </si>
+  <si>
+    <t>illness</t>
+  </si>
+  <si>
+    <t>0, No | 1, Yes, fever and rash | 2, Yes, other (specify) | 3, Yes, respiratory infection | 4, Yes, watery diarrhoea</t>
+  </si>
+  <si>
+    <t>ilness_other</t>
+  </si>
+  <si>
+    <t>0, Diarrhea, fever and rash | 1, died before</t>
+  </si>
+  <si>
+    <t>oedema</t>
+  </si>
+  <si>
+    <t>0, No | 1, Unknown</t>
+  </si>
+  <si>
+    <t>muac</t>
+  </si>
+  <si>
+    <t>arrived</t>
+  </si>
+  <si>
+    <t>date_arrived</t>
+  </si>
+  <si>
+    <t>departed</t>
+  </si>
+  <si>
+    <t>date_departed</t>
+  </si>
+  <si>
+    <t>born</t>
+  </si>
+  <si>
+    <t>date_born</t>
+  </si>
+  <si>
+    <t>died</t>
+  </si>
+  <si>
+    <t>date_died</t>
+  </si>
+  <si>
+    <t>cause_death</t>
+  </si>
+  <si>
+    <t>0, Fever | 1, Other (specify)</t>
+  </si>
+  <si>
+    <t>cause_death_other</t>
+  </si>
+  <si>
+    <t>0, Cancer | 1, Gunshot | 2, Stroke</t>
+  </si>
+  <si>
+    <t>indirect_identifier</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,10 +182,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <b/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,6 +217,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -481,25 +507,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" showGridLines="1" tabSelected="true">
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="11.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="10.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="141.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="8.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="6.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="113.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,44 +545,48 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2"/>
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2"/>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3"/>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3"/>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4"/>
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -568,12 +599,14 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5"/>
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -586,12 +619,14 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6"/>
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -604,12 +639,14 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7"/>
       <c r="C7" t="s">
         <v>13</v>
       </c>
@@ -622,12 +659,14 @@
       <c r="F7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="G7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8"/>
       <c r="C8" t="s">
         <v>13</v>
       </c>
@@ -640,12 +679,14 @@
       <c r="F8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9"/>
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -658,42 +699,45 @@
       <c r="F9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10"/>
       <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10"/>
       <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="G11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12"/>
       <c r="C12" t="s">
         <v>13</v>
       </c>
@@ -706,12 +750,14 @@
       <c r="F12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B13"/>
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -724,12 +770,14 @@
       <c r="F13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14"/>
       <c r="C14" t="s">
         <v>13</v>
       </c>
@@ -742,28 +790,31 @@
       <c r="F14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15"/>
       <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="D15"/>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16"/>
       <c r="C16" t="s">
         <v>13</v>
       </c>
@@ -776,28 +827,31 @@
       <c r="F16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B17"/>
       <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17"/>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B18"/>
       <c r="C18" t="s">
         <v>13</v>
       </c>
@@ -810,28 +864,31 @@
       <c r="F18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>37</v>
       </c>
-      <c r="B19"/>
       <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19"/>
       <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="G19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B20"/>
       <c r="C20" t="s">
         <v>13</v>
       </c>
@@ -844,28 +901,31 @@
       <c r="F20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="G20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21"/>
       <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21"/>
       <c r="E21" t="s">
         <v>8</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B22"/>
       <c r="C22" t="s">
         <v>13</v>
       </c>
@@ -878,28 +938,31 @@
       <c r="F22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="G22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>41</v>
       </c>
-      <c r="B23"/>
       <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23"/>
       <c r="E23" t="s">
         <v>8</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="G23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
-      <c r="B24"/>
       <c r="C24" t="s">
         <v>13</v>
       </c>
@@ -912,12 +975,14 @@
       <c r="F24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="G24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B25"/>
       <c r="C25" t="s">
         <v>13</v>
       </c>
@@ -930,9 +995,12 @@
       <c r="F25" t="s">
         <v>9</v>
       </c>
+      <c r="G25" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>